<commit_message>
checkpoint before proof reading
</commit_message>
<xml_diff>
--- a/reports/06.99 Optimization Metrics.xlsx
+++ b/reports/06.99 Optimization Metrics.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmhenn/Documents/GitHub/Incident-Management-Process-BPIC2014/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43336292-A937-D648-98CE-9BCF32912857}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455E0108-FDDD-0242-BC08-105337BD34F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3060" windowWidth="31560" windowHeight="20460"/>
+    <workbookView xWindow="5400" yWindow="1980" windowWidth="31560" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="06.00 Optimization Metrics" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
   <si>
     <t>Optimize 1</t>
   </si>
@@ -334,13 +334,20 @@
   <si>
     <t>p-value</t>
   </si>
+  <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="18">
     <font>
@@ -819,12 +826,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1179,20 +1187,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5:X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
     <col min="12" max="12" width="26.6640625" customWidth="1"/>
+    <col min="22" max="22" width="28.5" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:24">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1206,7 +1216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1217,7 +1227,7 @@
         <v>0.70481870680677805</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:24" ht="409.6">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1234,7 +1244,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:24" ht="68">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1256,14 +1266,20 @@
       <c r="R4" t="s">
         <v>64</v>
       </c>
-      <c r="S4" t="s">
+      <c r="U4" t="s">
+        <v>68</v>
+      </c>
+      <c r="V4" t="s">
+        <v>67</v>
+      </c>
+      <c r="W4" t="s">
         <v>65</v>
       </c>
-      <c r="T4" t="s">
+      <c r="X4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1303,8 +1319,20 @@
       <c r="S5" s="2">
         <v>1.4728299999999999E-32</v>
       </c>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="U5" t="s">
+        <v>55</v>
+      </c>
+      <c r="V5" s="3">
+        <v>0.104001</v>
+      </c>
+      <c r="W5" s="3">
+        <v>141.584</v>
+      </c>
+      <c r="X5" s="3">
+        <v>1.4728299999999999E-32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1344,8 +1372,20 @@
       <c r="S6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="U6" t="s">
+        <v>56</v>
+      </c>
+      <c r="V6" s="3">
+        <v>0.18806400000000001</v>
+      </c>
+      <c r="W6" s="3">
+        <v>6104.44</v>
+      </c>
+      <c r="X6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1385,8 +1425,20 @@
       <c r="S7" s="2">
         <v>2.06821E-40</v>
       </c>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="U7" t="s">
+        <v>57</v>
+      </c>
+      <c r="V7" s="3">
+        <v>1.1217349999999999</v>
+      </c>
+      <c r="W7" s="3">
+        <v>177.756</v>
+      </c>
+      <c r="X7" s="3">
+        <v>2.06821E-40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1426,8 +1478,20 @@
       <c r="S8" s="2">
         <v>7.6138200000000004E-148</v>
       </c>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="U8" t="s">
+        <v>58</v>
+      </c>
+      <c r="V8" s="3">
+        <v>1.1726289999999999</v>
+      </c>
+      <c r="W8" s="3">
+        <v>679.76300000000003</v>
+      </c>
+      <c r="X8" s="3">
+        <v>7.6138200000000004E-148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1467,8 +1531,20 @@
       <c r="S9" s="2">
         <v>1.1003599999999999E-194</v>
       </c>
-    </row>
-    <row r="10" spans="1:20">
+      <c r="U9" t="s">
+        <v>59</v>
+      </c>
+      <c r="V9" s="3">
+        <v>1.2459340000000001</v>
+      </c>
+      <c r="W9" s="3">
+        <v>902.10900000000004</v>
+      </c>
+      <c r="X9" s="3">
+        <v>1.1003599999999999E-194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1508,8 +1584,20 @@
       <c r="S10" s="2">
         <v>3.4407000000000001E-15</v>
       </c>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="U10" t="s">
+        <v>60</v>
+      </c>
+      <c r="V10" s="3">
+        <v>3.882E-2</v>
+      </c>
+      <c r="W10" s="3">
+        <v>62.075800000000001</v>
+      </c>
+      <c r="X10" s="3">
+        <v>3.4407000000000001E-15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1549,8 +1637,20 @@
       <c r="S11" s="2">
         <v>1.7894299999999998E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="U11" t="s">
+        <v>61</v>
+      </c>
+      <c r="V11" s="3">
+        <v>0.18243599999999999</v>
+      </c>
+      <c r="W11" s="3">
+        <v>5.6072199999999999</v>
+      </c>
+      <c r="X11" s="3">
+        <v>1.7894299999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="221">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1590,8 +1690,20 @@
       <c r="S12" s="2">
         <v>0.55302499999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="U12" t="s">
+        <v>62</v>
+      </c>
+      <c r="V12" s="3">
+        <v>-3.5749999999999997E-2</v>
+      </c>
+      <c r="W12" s="3">
+        <v>0.351935</v>
+      </c>
+      <c r="X12" s="3">
+        <v>0.55302499999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="221">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1608,7 +1720,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:24" ht="409.6">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1622,7 +1734,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:24">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1636,7 +1748,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="409.6">
+    <row r="16" spans="1:24" ht="409.6">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1661,7 +1773,7 @@
         <v>-0.91615466660171896</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" ht="409.6">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -1705,7 +1817,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" ht="409.6">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -1729,7 +1841,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" ht="153">
       <c r="A25" t="s">
         <v>53</v>
       </c>

</xml_diff>